<commit_message>
Redid part 1 values
</commit_message>
<xml_diff>
--- a/Lab3/Lab 3.xlsx
+++ b/Lab3/Lab 3.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rit0-my.sharepoint.com/personal/twh4619_rit_edu/Documents/Year 3 (2024 - 2025)/Interface and Digital Electronics/IDELabs/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{19E50E6A-9F69-4C31-A6FF-2E685929E193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2A471A5-4B5B-476B-8989-2FA48705FEAE}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{19E50E6A-9F69-4C31-A6FF-2E685929E193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D162285F-1BC1-449E-B965-D845FE9D74FC}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{30B0A469-1ABF-4316-ACC0-52FC7C3B041A}"/>
   </bookViews>
   <sheets>
     <sheet name="Prelab" sheetId="1" r:id="rId1"/>
-    <sheet name="Part 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Part 1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -175,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -293,15 +293,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -324,7 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -343,6 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1290,73 +1281,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>3.92</c:v>
+                  <c:v>4.9189999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9969999999999999</c:v>
+                  <c:v>3.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0439999999999996</c:v>
+                  <c:v>0.72699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0620000000000003</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0839999999999996</c:v>
+                  <c:v>0.72899999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0869999999999997</c:v>
+                  <c:v>0.77100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0880000000000001</c:v>
+                  <c:v>0.81699999999999995</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.08</c:v>
+                  <c:v>1.6519999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0659999999999998</c:v>
+                  <c:v>2.5630000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0540000000000003</c:v>
+                  <c:v>3.1259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0540000000000003</c:v>
+                  <c:v>3.42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.05</c:v>
+                  <c:v>3.871</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0449999999999999</c:v>
+                  <c:v>4.0380000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.05</c:v>
+                  <c:v>4.2167000000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.08</c:v>
+                  <c:v>4.274</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1130000000000004</c:v>
+                  <c:v>4.319</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.2939999999999996</c:v>
+                  <c:v>4.5759999999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.4569999999999999</c:v>
+                  <c:v>4.6559999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.516</c:v>
+                  <c:v>4.641</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.548</c:v>
+                  <c:v>4.58</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.57</c:v>
+                  <c:v>4.5060000000000002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.5730000000000004</c:v>
+                  <c:v>4.5229999999999997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.5609999999999999</c:v>
+                  <c:v>4.585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1364,7 +1355,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B131-455C-92B4-90E480A27167}"/>
+              <c16:uniqueId val="{00000000-A9BD-4E5B-A762-A2AAB1F2FF93}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1753,73 +1744,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.10769844435580377</c:v>
+                  <c:v>8.0773833266853234E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10001994415636221</c:v>
+                  <c:v>0.1819904268049462</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5333067411248557E-2</c:v>
+                  <c:v>0.42610690067810136</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.3538093338651762E-2</c:v>
+                  <c:v>0.42780215396888716</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1344236138811374E-2</c:v>
+                  <c:v>0.42590745911447953</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.1045073793378575E-2</c:v>
+                  <c:v>0.42171918627842048</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0945353011567615E-2</c:v>
+                  <c:v>0.4171320303151177</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.1743119266055051E-2</c:v>
+                  <c:v>0.33386517750299166</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3139210211408086E-2</c:v>
+                  <c:v>0.24301954527323497</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.4335859593139199E-2</c:v>
+                  <c:v>0.18687674511368171</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.4335859593139199E-2</c:v>
+                  <c:v>0.15755883526126849</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.4734742720382958E-2</c:v>
+                  <c:v>0.1125847626645393</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.5233346629437596E-2</c:v>
+                  <c:v>9.5931392102114071E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.4734742720382958E-2</c:v>
+                  <c:v>7.8111288392500977E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.1743119266055051E-2</c:v>
+                  <c:v>7.2397287594734752E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.8452333466294344E-2</c:v>
+                  <c:v>6.7909852413242933E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.0402871958516203E-2</c:v>
+                  <c:v>4.228161148783411E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4148384523334682E-2</c:v>
+                  <c:v>3.4303948942959746E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.8264858396489835E-2</c:v>
+                  <c:v>3.5799760670123658E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.5073793378540089E-2</c:v>
+                  <c:v>4.1882728360590343E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.2879936178699618E-2</c:v>
+                  <c:v>4.926206621459911E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.2580773833266819E-2</c:v>
+                  <c:v>4.7566812923813359E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.3777423214998015E-2</c:v>
+                  <c:v>4.1384124451535706E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1827,7 +1818,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2CB8-4571-A236-F29D093AF942}"/>
+              <c16:uniqueId val="{00000000-8C43-4FED-BAF0-1BED52BE68A4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2216,73 +2207,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>2.62</c:v>
+                  <c:v>4.8099999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.718</c:v>
+                  <c:v>1.2250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7919999999999998</c:v>
+                  <c:v>0.73719999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.85</c:v>
+                  <c:v>0.69840000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.91</c:v>
+                  <c:v>0.68310000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9470000000000001</c:v>
+                  <c:v>0.68740000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.96</c:v>
+                  <c:v>0.69710000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9910000000000001</c:v>
+                  <c:v>0.71560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0139999999999998</c:v>
+                  <c:v>0.73499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0289999999999999</c:v>
+                  <c:v>0.75139999999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0510000000000002</c:v>
+                  <c:v>0.76500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0579999999999998</c:v>
+                  <c:v>0.78990000000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0550000000000002</c:v>
+                  <c:v>0.80589999999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0409999999999999</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0190000000000001</c:v>
+                  <c:v>0.88019999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.0019999999999998</c:v>
+                  <c:v>1.3460000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.19</c:v>
+                  <c:v>3.43</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.6059999999999999</c:v>
+                  <c:v>4.0780000000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.85</c:v>
+                  <c:v>4.2430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.984</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.0730000000000004</c:v>
+                  <c:v>4.0430000000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.1280000000000001</c:v>
+                  <c:v>4.0179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.1520000000000001</c:v>
+                  <c:v>4.0815000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2290,7 +2281,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FD65-42E2-8F4C-DBB64B80A492}"/>
+              <c16:uniqueId val="{00000000-6A47-481B-9A90-791B0DD47E6C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2679,73 +2670,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.11852589641434264</c:v>
+                  <c:v>9.4621513944223318E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.11364541832669324</c:v>
+                  <c:v>0.18799800796812749</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10996015936254983</c:v>
+                  <c:v>0.21229083665338649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10707171314741036</c:v>
+                  <c:v>0.21422310756972113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10408366533864542</c:v>
+                  <c:v>0.21498505976095622</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10224103585657371</c:v>
+                  <c:v>0.21477091633466136</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10159362549800798</c:v>
+                  <c:v>0.2142878486055777</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10004980079681275</c:v>
+                  <c:v>0.21336653386454185</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.890438247011954E-2</c:v>
+                  <c:v>0.21240039840637451</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8157370517928305E-2</c:v>
+                  <c:v>0.21158366533864542</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.7061752988047811E-2</c:v>
+                  <c:v>0.21090637450199207</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.671314741035858E-2</c:v>
+                  <c:v>0.20966633466135459</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.686254980079681E-2</c:v>
+                  <c:v>0.20886952191235061</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.7559760956175315E-2</c:v>
+                  <c:v>0.20816733067729085</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.8655378486055781E-2</c:v>
+                  <c:v>0.20516932270916335</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.950199203187253E-2</c:v>
+                  <c:v>0.18197211155378487</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0139442231075714E-2</c:v>
+                  <c:v>7.8187250996015936E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.9422310756972125E-2</c:v>
+                  <c:v>4.5916334661354571E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.7270916334661352E-2</c:v>
+                  <c:v>3.7699203187250986E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.0597609561752993E-2</c:v>
+                  <c:v>3.9840637450199196E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.6165338645418309E-2</c:v>
+                  <c:v>4.7659362549800792E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.342629482071713E-2</c:v>
+                  <c:v>4.8904382470119537E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.223107569721115E-2</c:v>
+                  <c:v>4.5742031872509956E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2753,7 +2744,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C5B5-41A7-910B-CEFA8A06D794}"/>
+              <c16:uniqueId val="{00000000-BAC0-453C-A67D-F81F7CDCD040}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6377,11 +6368,13 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A85DC37-7375-9F71-D243-F1492329CCD5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1988BF22-8CC8-46B8-80E1-B35FC20A132F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6413,11 +6406,13 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF82B51-62F1-6032-5172-581556B0F7B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27144055-A5B4-42DC-AC3C-34D902BF38F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6449,11 +6444,13 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB35702D-64DA-3BC4-9603-BC642C4A9177}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24BEF751-0602-4D38-852C-3CF1D6658EFA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6485,11 +6482,13 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A4168F-1CA9-F76E-BC99-EB3EF1FC3F7B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F8B254F-CDF1-4C00-99F9-0E122C003E69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -6504,6 +6503,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6832,12 +6835,12 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="13"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
@@ -7018,11 +7021,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B2CA89-4C23-4038-B0F6-2B75D1E8FCF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379240FB-D1B7-44EE-909B-4319BEE6CAD3}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7032,14 +7035,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="5"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
@@ -7048,13 +7051,13 @@
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -7063,18 +7066,18 @@
         <v>0</v>
       </c>
       <c r="B3" s="6">
-        <v>3.92</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C25" si="0">(5-B3)/(8.068+1.96)</f>
-        <v>0.10769844435580377</v>
+        <v>4.9189999999999996</v>
+      </c>
+      <c r="C3" s="17">
+        <f>(5-B3)/(8.068+1.96)</f>
+        <v>8.0773833266853234E-3</v>
       </c>
       <c r="D3" s="6">
-        <v>2.62</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="E3" s="7">
         <f>(5-D3)/((8.068+1.96+8.079+1.973))</f>
-        <v>0.11852589641434264</v>
+        <v>9.4621513944223318E-3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
@@ -7082,18 +7085,18 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>3.9969999999999999</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>0.10001994415636221</v>
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="C4" s="17">
+        <f t="shared" ref="C4:C25" si="0">(5-B4)/(8.068+1.96)</f>
+        <v>0.1819904268049462</v>
       </c>
       <c r="D4" s="6">
-        <v>2.718</v>
+        <v>1.2250000000000001</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" ref="E4:E25" si="1">(5-D4)/((8.068+1.96+8.079+1.973))</f>
-        <v>0.11364541832669324</v>
+        <v>0.18799800796812749</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -7101,18 +7104,18 @@
         <v>2</v>
       </c>
       <c r="B5" s="6">
-        <v>4.0439999999999996</v>
-      </c>
-      <c r="C5">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="C5" s="17">
         <f t="shared" si="0"/>
-        <v>9.5333067411248557E-2</v>
+        <v>0.42610690067810136</v>
       </c>
       <c r="D5" s="6">
-        <v>2.7919999999999998</v>
+        <v>0.73719999999999997</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="1"/>
-        <v>0.10996015936254983</v>
+        <v>0.21229083665338649</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
@@ -7120,18 +7123,18 @@
         <v>3</v>
       </c>
       <c r="B6" s="6">
-        <v>4.0620000000000003</v>
-      </c>
-      <c r="C6">
+        <v>0.71</v>
+      </c>
+      <c r="C6" s="17">
         <f t="shared" si="0"/>
-        <v>9.3538093338651762E-2</v>
+        <v>0.42780215396888716</v>
       </c>
       <c r="D6" s="6">
-        <v>2.85</v>
+        <v>0.69840000000000002</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="1"/>
-        <v>0.10707171314741036</v>
+        <v>0.21422310756972113</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -7139,18 +7142,18 @@
         <v>4</v>
       </c>
       <c r="B7" s="6">
-        <v>4.0839999999999996</v>
-      </c>
-      <c r="C7">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="C7" s="17">
         <f t="shared" si="0"/>
-        <v>9.1344236138811374E-2</v>
+        <v>0.42590745911447953</v>
       </c>
       <c r="D7" s="6">
-        <v>2.91</v>
+        <v>0.68310000000000004</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="1"/>
-        <v>0.10408366533864542</v>
+        <v>0.21498505976095622</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
@@ -7158,18 +7161,18 @@
         <v>5</v>
       </c>
       <c r="B8" s="6">
-        <v>4.0869999999999997</v>
-      </c>
-      <c r="C8">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="C8" s="17">
         <f t="shared" si="0"/>
-        <v>9.1045073793378575E-2</v>
+        <v>0.42171918627842048</v>
       </c>
       <c r="D8" s="6">
-        <v>2.9470000000000001</v>
+        <v>0.68740000000000001</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>0.10224103585657371</v>
+        <v>0.21477091633466136</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
@@ -7177,18 +7180,18 @@
         <v>6</v>
       </c>
       <c r="B9" s="6">
-        <v>4.0880000000000001</v>
-      </c>
-      <c r="C9">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="C9" s="17">
         <f t="shared" si="0"/>
-        <v>9.0945353011567615E-2</v>
+        <v>0.4171320303151177</v>
       </c>
       <c r="D9" s="6">
-        <v>2.96</v>
+        <v>0.69710000000000005</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="1"/>
-        <v>0.10159362549800798</v>
+        <v>0.2142878486055777</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -7196,18 +7199,18 @@
         <v>7</v>
       </c>
       <c r="B10" s="6">
-        <v>4.08</v>
-      </c>
-      <c r="C10">
+        <v>1.6519999999999999</v>
+      </c>
+      <c r="C10" s="17">
         <f t="shared" si="0"/>
-        <v>9.1743119266055051E-2</v>
+        <v>0.33386517750299166</v>
       </c>
       <c r="D10" s="6">
-        <v>2.9910000000000001</v>
+        <v>0.71560000000000001</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="1"/>
-        <v>0.10004980079681275</v>
+        <v>0.21336653386454185</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
@@ -7215,18 +7218,18 @@
         <v>8</v>
       </c>
       <c r="B11" s="6">
-        <v>4.0659999999999998</v>
-      </c>
-      <c r="C11">
+        <v>2.5630000000000002</v>
+      </c>
+      <c r="C11" s="17">
         <f t="shared" si="0"/>
-        <v>9.3139210211408086E-2</v>
+        <v>0.24301954527323497</v>
       </c>
       <c r="D11" s="6">
-        <v>3.0139999999999998</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="1"/>
-        <v>9.890438247011954E-2</v>
+        <v>0.21240039840637451</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
@@ -7234,18 +7237,18 @@
         <v>9</v>
       </c>
       <c r="B12" s="6">
-        <v>4.0540000000000003</v>
-      </c>
-      <c r="C12">
+        <v>3.1259999999999999</v>
+      </c>
+      <c r="C12" s="17">
         <f t="shared" si="0"/>
-        <v>9.4335859593139199E-2</v>
+        <v>0.18687674511368171</v>
       </c>
       <c r="D12" s="6">
-        <v>3.0289999999999999</v>
+        <v>0.75139999999999996</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="1"/>
-        <v>9.8157370517928305E-2</v>
+        <v>0.21158366533864542</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
@@ -7253,18 +7256,18 @@
         <v>10</v>
       </c>
       <c r="B13" s="6">
-        <v>4.0540000000000003</v>
-      </c>
-      <c r="C13">
+        <v>3.42</v>
+      </c>
+      <c r="C13" s="17">
         <f t="shared" si="0"/>
-        <v>9.4335859593139199E-2</v>
+        <v>0.15755883526126849</v>
       </c>
       <c r="D13" s="6">
-        <v>3.0510000000000002</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="1"/>
-        <v>9.7061752988047811E-2</v>
+        <v>0.21090637450199207</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -7272,18 +7275,18 @@
         <v>11</v>
       </c>
       <c r="B14" s="6">
-        <v>4.05</v>
-      </c>
-      <c r="C14">
+        <v>3.871</v>
+      </c>
+      <c r="C14" s="17">
         <f t="shared" si="0"/>
-        <v>9.4734742720382958E-2</v>
+        <v>0.1125847626645393</v>
       </c>
       <c r="D14" s="6">
-        <v>3.0579999999999998</v>
+        <v>0.78990000000000005</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="1"/>
-        <v>9.671314741035858E-2</v>
+        <v>0.20966633466135459</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
@@ -7291,18 +7294,18 @@
         <v>12</v>
       </c>
       <c r="B15" s="6">
-        <v>4.0449999999999999</v>
-      </c>
-      <c r="C15">
+        <v>4.0380000000000003</v>
+      </c>
+      <c r="C15" s="17">
         <f t="shared" si="0"/>
-        <v>9.5233346629437596E-2</v>
+        <v>9.5931392102114071E-2</v>
       </c>
       <c r="D15" s="6">
-        <v>3.0550000000000002</v>
+        <v>0.80589999999999995</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="1"/>
-        <v>9.686254980079681E-2</v>
+        <v>0.20886952191235061</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
@@ -7310,18 +7313,18 @@
         <v>13</v>
       </c>
       <c r="B16" s="6">
-        <v>4.05</v>
-      </c>
-      <c r="C16">
+        <v>4.2167000000000003</v>
+      </c>
+      <c r="C16" s="17">
         <f t="shared" si="0"/>
-        <v>9.4734742720382958E-2</v>
+        <v>7.8111288392500977E-2</v>
       </c>
       <c r="D16" s="6">
-        <v>3.0409999999999999</v>
+        <v>0.82</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="1"/>
-        <v>9.7559760956175315E-2</v>
+        <v>0.20816733067729085</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -7329,18 +7332,18 @@
         <v>14</v>
       </c>
       <c r="B17" s="6">
-        <v>4.08</v>
-      </c>
-      <c r="C17">
+        <v>4.274</v>
+      </c>
+      <c r="C17" s="17">
         <f t="shared" si="0"/>
-        <v>9.1743119266055051E-2</v>
+        <v>7.2397287594734752E-2</v>
       </c>
       <c r="D17" s="6">
-        <v>3.0190000000000001</v>
+        <v>0.88019999999999998</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="1"/>
-        <v>9.8655378486055781E-2</v>
+        <v>0.20516932270916335</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -7348,18 +7351,18 @@
         <v>15</v>
       </c>
       <c r="B18" s="6">
-        <v>4.1130000000000004</v>
-      </c>
-      <c r="C18">
+        <v>4.319</v>
+      </c>
+      <c r="C18" s="17">
         <f t="shared" si="0"/>
-        <v>8.8452333466294344E-2</v>
+        <v>6.7909852413242933E-2</v>
       </c>
       <c r="D18" s="6">
-        <v>3.0019999999999998</v>
+        <v>1.3460000000000001</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="1"/>
-        <v>9.950199203187253E-2</v>
+        <v>0.18197211155378487</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -7367,18 +7370,18 @@
         <v>20</v>
       </c>
       <c r="B19" s="6">
-        <v>4.2939999999999996</v>
-      </c>
-      <c r="C19">
+        <v>4.5759999999999996</v>
+      </c>
+      <c r="C19" s="17">
         <f t="shared" si="0"/>
-        <v>7.0402871958516203E-2</v>
+        <v>4.228161148783411E-2</v>
       </c>
       <c r="D19" s="6">
-        <v>3.19</v>
+        <v>3.43</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="1"/>
-        <v>9.0139442231075714E-2</v>
+        <v>7.8187250996015936E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -7386,18 +7389,18 @@
         <v>25</v>
       </c>
       <c r="B20" s="6">
-        <v>4.4569999999999999</v>
-      </c>
-      <c r="C20">
+        <v>4.6559999999999997</v>
+      </c>
+      <c r="C20" s="17">
         <f t="shared" si="0"/>
-        <v>5.4148384523334682E-2</v>
+        <v>3.4303948942959746E-2</v>
       </c>
       <c r="D20" s="6">
-        <v>3.6059999999999999</v>
+        <v>4.0780000000000003</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="1"/>
-        <v>6.9422310756972125E-2</v>
+        <v>4.5916334661354571E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -7405,18 +7408,18 @@
         <v>30</v>
       </c>
       <c r="B21" s="6">
-        <v>4.516</v>
-      </c>
-      <c r="C21">
+        <v>4.641</v>
+      </c>
+      <c r="C21" s="17">
         <f t="shared" si="0"/>
-        <v>4.8264858396489835E-2</v>
+        <v>3.5799760670123658E-2</v>
       </c>
       <c r="D21" s="6">
-        <v>3.85</v>
+        <v>4.2430000000000003</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="1"/>
-        <v>5.7270916334661352E-2</v>
+        <v>3.7699203187250986E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -7424,18 +7427,18 @@
         <v>35</v>
       </c>
       <c r="B22" s="6">
-        <v>4.548</v>
-      </c>
-      <c r="C22">
+        <v>4.58</v>
+      </c>
+      <c r="C22" s="17">
         <f t="shared" si="0"/>
-        <v>4.5073793378540089E-2</v>
+        <v>4.1882728360590343E-2</v>
       </c>
       <c r="D22" s="6">
-        <v>3.984</v>
+        <v>4.2</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="1"/>
-        <v>5.0597609561752993E-2</v>
+        <v>3.9840637450199196E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -7443,18 +7446,18 @@
         <v>40</v>
       </c>
       <c r="B23" s="6">
-        <v>4.57</v>
-      </c>
-      <c r="C23">
+        <v>4.5060000000000002</v>
+      </c>
+      <c r="C23" s="17">
         <f t="shared" si="0"/>
-        <v>4.2879936178699618E-2</v>
+        <v>4.926206621459911E-2</v>
       </c>
       <c r="D23" s="6">
-        <v>4.0730000000000004</v>
+        <v>4.0430000000000001</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="1"/>
-        <v>4.6165338645418309E-2</v>
+        <v>4.7659362549800792E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -7462,18 +7465,18 @@
         <v>45</v>
       </c>
       <c r="B24" s="6">
-        <v>4.5730000000000004</v>
-      </c>
-      <c r="C24">
+        <v>4.5229999999999997</v>
+      </c>
+      <c r="C24" s="17">
         <f t="shared" si="0"/>
-        <v>4.2580773833266819E-2</v>
+        <v>4.7566812923813359E-2</v>
       </c>
       <c r="D24" s="6">
-        <v>4.1280000000000001</v>
+        <v>4.0179999999999998</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="1"/>
-        <v>4.342629482071713E-2</v>
+        <v>4.8904382470119537E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -7481,18 +7484,18 @@
         <v>50</v>
       </c>
       <c r="B25" s="8">
-        <v>4.5609999999999999</v>
+        <v>4.585</v>
       </c>
       <c r="C25" s="9">
         <f t="shared" si="0"/>
-        <v>4.3777423214998015E-2</v>
+        <v>4.1384124451535706E-2</v>
       </c>
       <c r="D25" s="8">
-        <v>4.1520000000000001</v>
-      </c>
-      <c r="E25" s="10">
+        <v>4.0815000000000001</v>
+      </c>
+      <c r="E25" s="9">
         <f t="shared" si="1"/>
-        <v>4.223107569721115E-2</v>
+        <v>4.5742031872509956E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>